<commit_message>
finished meeting minutes for 2/10
</commit_message>
<xml_diff>
--- a/Spring2016/2016 CSEC GBM 1 [2-10].xlsx
+++ b/Spring2016/2016 CSEC GBM 1 [2-10].xlsx
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>CSEC GBM 2</t>
   </si>
@@ -74,9 +74,6 @@
   </si>
   <si>
     <t>Useful Links</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>Bash Scripting</t>
@@ -113,6 +110,27 @@
   </si>
   <si>
     <t>&lt;- apt-get install sl</t>
+  </si>
+  <si>
+    <t>Bash Scripting Presentation</t>
+  </si>
+  <si>
+    <t>Can use command line program calls in bash scripting</t>
+  </si>
+  <si>
+    <t>Makes automation of programs easy since you don’t have to reimplement protocols</t>
+  </si>
+  <si>
+    <t>Example: openssl</t>
+  </si>
+  <si>
+    <t>Bash: call openssl with commandline arguments</t>
+  </si>
+  <si>
+    <t>Other: import openssl libraries and use various fucntion calls that vary</t>
+  </si>
+  <si>
+    <t>between languages</t>
   </si>
 </sst>
 </file>
@@ -354,6 +372,95 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectangle 1" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12700000" cy="12700000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1054100</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>186558</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5232400" y="1710558"/>
+          <a:ext cx="4279900" cy="2645542"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -624,8 +731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -660,7 +767,7 @@
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="25" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F2" s="9"/>
     </row>
@@ -674,7 +781,7 @@
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F3" s="9"/>
     </row>
@@ -684,7 +791,7 @@
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
       <c r="E4" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F4" s="9"/>
     </row>
@@ -693,11 +800,13 @@
         <v>6</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
+      <c r="E5" s="10" t="s">
+        <v>19</v>
+      </c>
       <c r="F5" s="9"/>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -705,7 +814,9 @@
       <c r="B6" s="15"/>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
-      <c r="E6" s="11"/>
+      <c r="E6" s="18" t="s">
+        <v>20</v>
+      </c>
       <c r="F6" s="16"/>
       <c r="G6" s="9"/>
     </row>
@@ -713,11 +824,17 @@
       <c r="A7" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="13"/>
+      <c r="B7" s="23" t="s">
+        <v>18</v>
+      </c>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="9"/>
+      <c r="E7" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>22</v>
+      </c>
       <c r="G7" s="9"/>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -726,7 +843,9 @@
       <c r="C8" s="6"/>
       <c r="D8" s="10"/>
       <c r="E8" s="11"/>
-      <c r="F8" s="9"/>
+      <c r="F8" s="18" t="s">
+        <v>23</v>
+      </c>
       <c r="G8" s="9"/>
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -737,24 +856,24 @@
       <c r="C9" s="6"/>
       <c r="D9" s="10"/>
       <c r="E9" s="11"/>
-      <c r="F9" s="9"/>
+      <c r="F9" s="18" t="s">
+        <v>24</v>
+      </c>
       <c r="G9" s="9"/>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" s="21"/>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
-      <c r="F10" s="9" t="s">
-        <v>9</v>
-      </c>
+      <c r="F10" s="9"/>
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="23" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" s="10"/>
       <c r="C11" s="10"/>
@@ -765,7 +884,7 @@
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="10"/>
@@ -776,10 +895,10 @@
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>17</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>18</v>
       </c>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
@@ -880,9 +999,10 @@
     <hyperlink ref="A11" r:id="rId2" display="In-Depth Manual"/>
     <hyperlink ref="A12" r:id="rId3"/>
     <hyperlink ref="A13" r:id="rId4"/>
+    <hyperlink ref="B7" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId5"/>
-  <legacyDrawing r:id="rId6"/>
+  <drawing r:id="rId6"/>
+  <legacyDrawing r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>